<commit_message>
Updated spreadsheet to include sources
Updated audit report spreadsheet to include sources for clarification
</commit_message>
<xml_diff>
--- a/site-audit/seo-audit-mike-final.xlsx
+++ b/site-audit/seo-audit-mike-final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\OpenClassroom\WD 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\OpenClassroom\WD 4\P4-Project-Updates\OC-Optimize-Existing-Website-SEO\site-audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06CC5D6-6948-4E3E-B487-3C7580EF707C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4846DE62-5C26-43E1-979D-C6D32FEADD37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10065" yWindow="0" windowWidth="18735" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Category</t>
   </si>
@@ -160,6 +160,37 @@
   </si>
   <si>
     <t>http://www.velizaratellalyan.com/seo/the-importance-of-bold-and-strong-tags-in-seo/</t>
+  </si>
+  <si>
+    <t>https://www.tmprod.com/blog/2010/h1-h2-and-h3-header-tags-for-seo/ https://www.w3schools.com/html/html5_semantic_elements.asp</t>
+  </si>
+  <si>
+    <t>https://ahrefs.com/blog/anchor-text/</t>
+  </si>
+  <si>
+    <t>https://cognitiveseo.com/blog/12169/44-black-hat-seo-techniques/#6</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-contrast.html</t>
+  </si>
+  <si>
+    <t>https://moz.com/learn/seo/alt-text 
+https://adolab.com/alt-text-best-practices-seo-mistakes/</t>
+  </si>
+  <si>
+    <t>https://adolab.com/alt-text-best-practices-seo-mistakes/
+https://adolab.com/what-is-image-alt-text-beginners-guide/</t>
+  </si>
+  <si>
+    <t>https://ahrefs.com/blog/image-seo/
+https://developers.google.com/search/docs/advanced/guidelines/google-images</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/advanced/guidelines/google-images/
+https://www.searchenginejournal.com/on-page-seo/image-optimization/</t>
+  </si>
+  <si>
+    <t>https://imageseo.io/images-seo-optimization/</t>
   </si>
 </sst>
 </file>
@@ -472,15 +503,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.77734375" customWidth="1"/>
-    <col min="6" max="6" width="48.88671875" customWidth="1"/>
+    <col min="6" max="6" width="64.33203125" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -552,7 +583,9 @@
       <c r="E3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -570,7 +603,9 @@
       <c r="E4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -588,7 +623,9 @@
       <c r="E5" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -606,7 +643,9 @@
       <c r="E6" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -624,7 +663,9 @@
       <c r="E7" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -642,7 +683,9 @@
       <c r="E8" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -680,7 +723,9 @@
       <c r="E10" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -698,7 +743,9 @@
       <c r="E11" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -716,7 +763,9 @@
       <c r="E12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -753,6 +802,13 @@
   <hyperlinks>
     <hyperlink ref="F9" r:id="rId1" display="https://www.w3.org/TR/html401/struct/dirlang.html" xr:uid="{20846C5E-5FEB-41EC-ABFC-3CAA39367043}"/>
     <hyperlink ref="F13" r:id="rId2" xr:uid="{245D913F-3F86-4D05-9D2D-618FAE55ABC4}"/>
+    <hyperlink ref="F12" r:id="rId3" display="https://www.tmprod.com/blog/2010/h1-h2-and-h3-header-tags-for-seo/" xr:uid="{24B3D42F-27F6-4D8A-9E6A-56458B161CCC}"/>
+    <hyperlink ref="F11" r:id="rId4" xr:uid="{E84D424D-1E64-45F3-BD76-1B0BEF806327}"/>
+    <hyperlink ref="F10" r:id="rId5" location="6" xr:uid="{7048C7BD-399F-443B-8576-DB96ABE7DBDE}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{628EC230-F8C4-40E3-9BF1-956007532203}"/>
+    <hyperlink ref="F7" r:id="rId7" display="https://moz.com/learn/seo/alt-text" xr:uid="{218D4275-59FA-4159-A61B-F5E0253F08A4}"/>
+    <hyperlink ref="F5" r:id="rId8" display="https://ahrefs.com/blog/image-seo/" xr:uid="{4E5B8303-E447-4D91-8017-57C089D2DF78}"/>
+    <hyperlink ref="F3" r:id="rId9" xr:uid="{3004D70F-B198-420B-8DFF-1C6D807B8EAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Updated bootstrap to latest version within 3 (3.4.1)
To address potential vulnerabilities the site has been updated to the latest version of Bootstrap 3.

Updated spreadsheet of changes for the audit
</commit_message>
<xml_diff>
--- a/site-audit/seo-audit-mike-final.xlsx
+++ b/site-audit/seo-audit-mike-final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\OpenClassroom\WD 4\P4-Project-Updates\OC-Optimize-Existing-Website-SEO\site-audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4846DE62-5C26-43E1-979D-C6D32FEADD37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A2BF4-40A4-4221-ACA8-A400FE236B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10065" yWindow="0" windowWidth="18735" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Category</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Using a descriptive filename provides google with easy to access information about the image.</t>
   </si>
   <si>
-    <t>Name each image with an appropiate name but keep it short, avoid keyword stuffing</t>
-  </si>
-  <si>
     <t>Image alt tags</t>
   </si>
   <si>
@@ -90,52 +87,28 @@
     <t xml:space="preserve">SEO </t>
   </si>
   <si>
-    <t>Accessability</t>
-  </si>
-  <si>
-    <t>Proper use of alt tags on imags allows users with visual disabilities to understand images without seeing them</t>
-  </si>
-  <si>
-    <t>Apply alt tags the properly describe the image without repeting or deviating from the image itself.</t>
-  </si>
-  <si>
     <t>contrast text/background</t>
   </si>
   <si>
     <t xml:space="preserve">Improper usage of colors makes a site difficult to use and will indirectly affect ranking due to a high bounce rate. </t>
   </si>
   <si>
-    <t>Choose background, foreground, and text colors that work together to maintain visability</t>
-  </si>
-  <si>
     <t>HTML Head</t>
   </si>
   <si>
-    <t>It is necessary to follow best practices here to improve SEO and Accessability</t>
-  </si>
-  <si>
     <t>Language should be identified. Meta tags should be refined to suit each use.</t>
   </si>
   <si>
-    <t>Accessability/SEO</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blackhat Keywords </t>
   </si>
   <si>
     <t>Adding keywords in the html without using them in context will result in penalization from Google</t>
   </si>
   <si>
-    <t>Incorperate keywords into the content in a natural way using proper context.</t>
-  </si>
-  <si>
     <t>Link text</t>
   </si>
   <si>
     <t>Links should be clear where they lead to and in the case of image links, an alt tag should be added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some links do not clearly describe where they go. This can impact SEO and accessability </t>
   </si>
   <si>
     <t>Semantic HTML</t>
@@ -178,10 +151,6 @@
 https://adolab.com/alt-text-best-practices-seo-mistakes/</t>
   </si>
   <si>
-    <t>https://adolab.com/alt-text-best-practices-seo-mistakes/
-https://adolab.com/what-is-image-alt-text-beginners-guide/</t>
-  </si>
-  <si>
     <t>https://ahrefs.com/blog/image-seo/
 https://developers.google.com/search/docs/advanced/guidelines/google-images</t>
   </si>
@@ -191,6 +160,53 @@
   </si>
   <si>
     <t>https://imageseo.io/images-seo-optimization/</t>
+  </si>
+  <si>
+    <t>Best Practices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To ensure site security, all dependencies should be kept up to date when possible. </t>
+  </si>
+  <si>
+    <t>Name each image with an appropriate name but keep it short, avoid keyword stuffing</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Proper use of alt tags on images allows users with visual disabilities to understand images without seeing them</t>
+  </si>
+  <si>
+    <t>Apply alt tags the properly describe the image without repeating or deviating from the image itself.</t>
+  </si>
+  <si>
+    <t>Choose background, foreground, and text colors that work together to maintain visibility</t>
+  </si>
+  <si>
+    <t>Accessibility/SEO</t>
+  </si>
+  <si>
+    <t>It is necessary to follow best practices here to improve SEO and Accessibility</t>
+  </si>
+  <si>
+    <t>Incorporate keywords into the content in a natural way using proper context.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some links do not clearly describe where they go. This can impact SEO and accessibility </t>
+  </si>
+  <si>
+    <t>Stay up to date on the current releases of dependencies within your project.</t>
+  </si>
+  <si>
+    <t>https://adolab.com/alt-text-best-practices-seo-mistakes/ 
+https://adolab.com/what-is-image-alt-text-beginners-guide/</t>
+  </si>
+  <si>
+    <t>jQuery Vesrion and Bootstrap Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/jquery/jquery-migrate/#README 
+https://getbootstrap.com/docs/versions/ </t>
   </si>
 </sst>
 </file>
@@ -503,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -584,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
@@ -604,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
@@ -618,93 +634,93 @@
         <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="E7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
@@ -712,19 +728,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
@@ -732,19 +748,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E11" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="75.75" x14ac:dyDescent="0.25">
@@ -752,19 +768,19 @@
         <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E12" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
@@ -772,31 +788,43 @@
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F13" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="F15" s="5"/>
+      <c r="F15" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -809,6 +837,7 @@
     <hyperlink ref="F7" r:id="rId7" display="https://moz.com/learn/seo/alt-text" xr:uid="{218D4275-59FA-4159-A61B-F5E0253F08A4}"/>
     <hyperlink ref="F5" r:id="rId8" display="https://ahrefs.com/blog/image-seo/" xr:uid="{4E5B8303-E447-4D91-8017-57C089D2DF78}"/>
     <hyperlink ref="F3" r:id="rId9" xr:uid="{3004D70F-B198-420B-8DFF-1C6D807B8EAB}"/>
+    <hyperlink ref="F14" r:id="rId10" location="README " display="https://github.com/jquery/jquery-migrate/#README " xr:uid="{65CB0A8B-8DCC-467A-8CC0-A73B3F2939FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Added final note to readme
</commit_message>
<xml_diff>
--- a/site-audit/seo-audit-mike-final.xlsx
+++ b/site-audit/seo-audit-mike-final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\OpenClassroom\WD 4\P4-Project-Updates\OC-Optimize-Existing-Website-SEO\site-audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A2BF4-40A4-4221-ACA8-A400FE236B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E26B02-C64A-419B-BE08-3DA8A762D90E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10065" yWindow="0" windowWidth="18735" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28995" yWindow="-7035" windowWidth="14895" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>